<commit_message>
11 may dsr update
</commit_message>
<xml_diff>
--- a/05_may_/May2023.xlsx
+++ b/05_may_/May2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="59">
   <si>
     <t>Day</t>
   </si>
@@ -109,10 +109,88 @@
     <t xml:space="preserve">apply another method on doble alert message when add special sale submit </t>
   </si>
   <si>
-    <t>try to add the add form modal on same page in store module in merchant side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add the add form page in store and add listing call after submit and close button working </t>
+    <t>try implement  to the add form modal on same page in store module in merchant side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add the add form page in store and add listing call after submit and close button working and apply disable button on post module  </t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>On leave</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Weekend Holiday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on the store add form modal and check there error or not </t>
+  </si>
+  <si>
+    <t>LMDI-37</t>
+  </si>
+  <si>
+    <t>email link not getting cause make notification for user registration and email templates N db</t>
+  </si>
+  <si>
+    <t>WBX-4555</t>
+  </si>
+  <si>
+    <t>try to figure out the solution of login on to the redirect to user route</t>
+  </si>
+  <si>
+    <t>add cancel button in add form in store module and update the code and merged the branch</t>
+  </si>
+  <si>
+    <t>work on the redirect through the email link splash screen disapear</t>
+  </si>
+  <si>
+    <t>reviewed pr of harshita</t>
+  </si>
+  <si>
+    <t>WBX-4582</t>
+  </si>
+  <si>
+    <t>work on the total earning issue where total earning blink</t>
+  </si>
+  <si>
+    <t>WBX-4595</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to power cut </t>
+  </si>
+  <si>
+    <t>WBX-4599</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test the user module and community module and special sale </t>
+  </si>
+  <si>
+    <t>WBX-4601</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try to solve the sorting issue in common nutrition in tracker module </t>
+  </si>
+  <si>
+    <t xml:space="preserve">due to office cleaning </t>
+  </si>
+  <si>
+    <t>WBX-4594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reviewd pr </t>
+  </si>
+  <si>
+    <t>try to find out the solution of listing issue</t>
+  </si>
+  <si>
+    <t>try to figure out the solution of listing issue where in order to asscending</t>
   </si>
 </sst>
 </file>
@@ -120,15 +198,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="mmm/yy"/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="mmm/yy"/>
     <numFmt numFmtId="182" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +237,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -167,8 +260,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,24 +282,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,15 +299,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,9 +308,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -258,16 +345,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,14 +368,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,7 +408,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,13 +444,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,19 +504,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,7 +546,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,108 +570,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -527,6 +613,195 @@
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -537,6 +812,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -556,63 +840,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -626,154 +853,154 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -808,11 +1035,67 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="5" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="5" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="5" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="12" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="13" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="14" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="179" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1133,10 +1416,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N38"/>
+  <dimension ref="A3:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1811,7 +2094,9 @@
     <row r="35" spans="1:14">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
-      <c r="C35" s="10"/>
+      <c r="C35" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="D35" s="8">
         <v>0.402777777777778</v>
       </c>
@@ -1833,7 +2118,9 @@
     <row r="36" spans="1:14">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="14"/>
+      <c r="C36" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D36" s="8">
         <v>0.458333333333333</v>
       </c>
@@ -1855,45 +2142,893 @@
     <row r="37" spans="1:14">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="14"/>
+      <c r="C37" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="D37" s="11">
         <v>0.0833333333333333</v>
       </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="9" t="s">
+      <c r="E37" s="11">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="10"/>
-      <c r="D38" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="E38" s="8">
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="30"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="18">
+        <v>45051</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="31"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="32"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="25"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="33"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="30"/>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="18">
+        <v>45052</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="31"/>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="21"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24"/>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="32"/>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="33"/>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="30"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="18">
+        <v>45053</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="31"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="21"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="24"/>
+      <c r="J56" s="24"/>
+      <c r="K56" s="24"/>
+      <c r="L56" s="24"/>
+      <c r="M56" s="24"/>
+      <c r="N56" s="32"/>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="25"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="28"/>
+      <c r="N57" s="33"/>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="6">
+        <v>45054</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E61" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E62" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E63" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="E64" s="8">
         <v>0.270833333333333</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
+      <c r="F64" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="34"/>
+      <c r="B65" s="34"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="6">
+        <v>45055</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E69" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E70" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="6"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E71" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E72" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="E73" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="6">
+        <v>45056</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E77" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D78" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E78" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79" s="11">
+        <v>0.194444444444444</v>
+      </c>
+      <c r="E79" s="8">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="6"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D80" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E80" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="A84" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5"/>
+      <c r="K84" s="5"/>
+      <c r="L84" s="5"/>
+      <c r="M84" s="5"/>
+      <c r="N84" s="5"/>
+    </row>
+    <row r="85" spans="1:14">
+      <c r="A85" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B85" s="6">
+        <v>45057</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E85" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
+    </row>
+    <row r="86" spans="1:14">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D86" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E86" s="8">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="9"/>
+    </row>
+    <row r="87" spans="1:14">
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87" s="8">
+        <v>0.444444444444444</v>
+      </c>
+      <c r="E87" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
+    </row>
+    <row r="88" spans="1:14">
+      <c r="A88" s="6"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D88" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E88" s="8">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
+    </row>
+    <row r="89" spans="1:14">
+      <c r="A89" s="35"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D89" s="8">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="E89" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
+    </row>
+    <row r="90" spans="1:14">
+      <c r="A90" s="35"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D90" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E90" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="83">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -1913,25 +3048,70 @@
     <mergeCell ref="F34:N34"/>
     <mergeCell ref="F35:N35"/>
     <mergeCell ref="F36:N36"/>
-    <mergeCell ref="F37:N37"/>
-    <mergeCell ref="F38:N38"/>
+    <mergeCell ref="C41:N41"/>
+    <mergeCell ref="C48:N48"/>
+    <mergeCell ref="C54:N54"/>
+    <mergeCell ref="F60:N60"/>
+    <mergeCell ref="F61:N61"/>
+    <mergeCell ref="F62:N62"/>
+    <mergeCell ref="F63:N63"/>
+    <mergeCell ref="F64:N64"/>
+    <mergeCell ref="F68:N68"/>
+    <mergeCell ref="F69:N69"/>
+    <mergeCell ref="F70:N70"/>
+    <mergeCell ref="F71:N71"/>
+    <mergeCell ref="F72:N72"/>
+    <mergeCell ref="F73:N73"/>
+    <mergeCell ref="F76:N76"/>
+    <mergeCell ref="F77:N77"/>
+    <mergeCell ref="F78:N78"/>
+    <mergeCell ref="F79:N79"/>
+    <mergeCell ref="F80:N80"/>
+    <mergeCell ref="F84:N84"/>
+    <mergeCell ref="F85:N85"/>
+    <mergeCell ref="F86:N86"/>
+    <mergeCell ref="F87:N87"/>
+    <mergeCell ref="F88:N88"/>
+    <mergeCell ref="F89:N89"/>
+    <mergeCell ref="F90:N90"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A77:A80"/>
+    <mergeCell ref="A85:A90"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B26:B30"/>
     <mergeCell ref="B34:B38"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="B85:B90"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D37:D38"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E37:E38"/>
     <mergeCell ref="C3:J4"/>
     <mergeCell ref="F11:N12"/>
     <mergeCell ref="F21:N22"/>
+    <mergeCell ref="F37:N38"/>
+    <mergeCell ref="C42:N44"/>
+    <mergeCell ref="C49:N51"/>
+    <mergeCell ref="C55:N57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
25 may 2023 dsr complete
</commit_message>
<xml_diff>
--- a/05_may_/May2023.xlsx
+++ b/05_may_/May2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="120">
   <si>
     <t>Day</t>
   </si>
@@ -271,7 +271,109 @@
     <t xml:space="preserve">rebase the branch and merged from faizan </t>
   </si>
   <si>
-    <t>test ui and check code status and raise pr</t>
+    <t>test ui and check code status and showed working pr</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>work on the browser tracker issue where  values changes</t>
+  </si>
+  <si>
+    <t>power cut</t>
+  </si>
+  <si>
+    <t>LMD-151</t>
+  </si>
+  <si>
+    <t>all hands meeting with sonia ma'am</t>
+  </si>
+  <si>
+    <t>work on the browser tracker issue where  values changes on cancel button</t>
+  </si>
+  <si>
+    <t>remove validation point in challenge add edit and value change on browser tracker</t>
+  </si>
+  <si>
+    <t>work on the commented code of sub goal and infographic and add to this challenge</t>
+  </si>
+  <si>
+    <t>WBX-4652</t>
+  </si>
+  <si>
+    <t>meeting with nidhi ma'am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try to solve the address validation issue where edit mode opened </t>
+  </si>
+  <si>
+    <t>start server run and take time  to start</t>
+  </si>
+  <si>
+    <t>worked on the update button disable in goal and map fields are shown for particular locale</t>
+  </si>
+  <si>
+    <t>WBX-4647</t>
+  </si>
+  <si>
+    <t>try to figureout the problem in notification view all pagination issue</t>
+  </si>
+  <si>
+    <t>WBX-4630</t>
+  </si>
+  <si>
+    <t>work store on the formatted address validation in edit mode and billing address using gapi</t>
+  </si>
+  <si>
+    <t>fix the limit skip and createdDate related issue in notification in backend</t>
+  </si>
+  <si>
+    <t>WBX-4651</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figureOut the problem pagination issue in notification </t>
+  </si>
+  <si>
+    <t>try to figureOut the problem in map listing related to particular selected locale</t>
+  </si>
+  <si>
+    <t>check working status and raise the pr and test on local</t>
+  </si>
+  <si>
+    <t>add to do on commented code in challenge add edit component and check  and raise pr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to office cleaning </t>
+  </si>
+  <si>
+    <t>localeids data share with challenge add edit to map component and update code</t>
+  </si>
+  <si>
+    <t>send the selected localeids to backend try to get the maplist based on the localeids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">try to figure Out the problem in particular localeids </t>
+  </si>
+  <si>
+    <t>WBX-4691</t>
+  </si>
+  <si>
+    <t>check changes and worked on the issue and create a map for localeId on local system</t>
+  </si>
+  <si>
+    <t>meeting with nidhi</t>
+  </si>
+  <si>
+    <t>restart server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figure out the problem in map list tried to solve them </t>
+  </si>
+  <si>
+    <t>take pull from official gitlab a/c and project setup for work N made changes there on local</t>
+  </si>
+  <si>
+    <t>work on the sorting related issue in common nutrition list</t>
   </si>
 </sst>
 </file>
@@ -279,15 +381,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="mmm/yy"/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="mmm/yy"/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="182" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,18 +429,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -349,7 +443,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,9 +457,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,6 +511,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -394,25 +526,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -424,24 +542,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -462,7 +571,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,25 +604,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFB4C6E7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,7 +628,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,19 +646,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,61 +700,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,7 +730,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,12 +748,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -834,22 +949,60 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -893,21 +1046,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -917,32 +1055,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -952,136 +1095,136 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="181" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1092,7 +1235,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1104,7 +1247,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1128,7 +1271,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="5" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="5" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="5" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,7 +1283,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="5" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="5" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="5" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1152,7 +1295,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="5" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="5" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="5" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1177,6 +1320,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="182" fontId="3" fillId="4" borderId="2" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="5" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1497,10 +1652,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:N152"/>
+  <dimension ref="A1:P213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="E158" sqref="E158"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="R211" sqref="R211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1512,6 +1667,7 @@
     <col min="5" max="5" width="13.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" customHeight="1"/>
     <row r="3" spans="3:10">
       <c r="C3" s="1">
         <v>45047</v>
@@ -3946,7 +4102,7 @@
     </row>
     <row r="137" spans="1:14">
       <c r="A137" s="6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B137" s="6">
         <v>45063</v>
@@ -4146,10 +4302,10 @@
     </row>
     <row r="147" spans="1:14">
       <c r="A147" s="6" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B147" s="6">
-        <v>45061</v>
+        <v>45064</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>72</v>
@@ -4196,7 +4352,7 @@
       <c r="M148" s="9"/>
       <c r="N148" s="9"/>
     </row>
-    <row r="149" spans="1:14">
+    <row r="149" spans="1:16">
       <c r="A149" s="6"/>
       <c r="B149" s="6"/>
       <c r="C149" s="7" t="s">
@@ -4219,14 +4375,25 @@
       <c r="L149" s="9"/>
       <c r="M149" s="9"/>
       <c r="N149" s="9"/>
+      <c r="P149" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="150" spans="1:14">
       <c r="A150" s="6"/>
       <c r="B150" s="6"/>
-      <c r="C150" s="35"/>
-      <c r="D150" s="8"/>
-      <c r="E150" s="8"/>
-      <c r="F150" s="9"/>
+      <c r="C150" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D150" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="E150" s="8">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="F150" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="G150" s="9"/>
       <c r="H150" s="9"/>
       <c r="I150" s="9"/>
@@ -4239,10 +4406,18 @@
     <row r="151" spans="1:14">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
-      <c r="C151" s="35"/>
-      <c r="D151" s="11"/>
-      <c r="E151" s="8"/>
-      <c r="F151" s="9"/>
+      <c r="C151" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D151" s="8">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="E151" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="G151" s="9"/>
       <c r="H151" s="9"/>
       <c r="I151" s="9"/>
@@ -4255,10 +4430,18 @@
     <row r="152" spans="1:14">
       <c r="A152" s="6"/>
       <c r="B152" s="6"/>
-      <c r="C152" s="7"/>
-      <c r="D152" s="8"/>
-      <c r="E152" s="8"/>
-      <c r="F152" s="9"/>
+      <c r="C152" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D152" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E152" s="8">
+        <v>0.197916666666667</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="G152" s="9"/>
       <c r="H152" s="9"/>
       <c r="I152" s="9"/>
@@ -4268,8 +4451,1144 @@
       <c r="M152" s="9"/>
       <c r="N152" s="9"/>
     </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="6"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D153" s="8">
+        <v>0.197916666666667</v>
+      </c>
+      <c r="E153" s="8">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9"/>
+      <c r="L153" s="9"/>
+      <c r="M153" s="9"/>
+      <c r="N153" s="9"/>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D154" s="8">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="E154" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G154" s="9"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="9"/>
+      <c r="J154" s="9"/>
+      <c r="K154" s="9"/>
+      <c r="L154" s="9"/>
+      <c r="M154" s="9"/>
+      <c r="N154" s="9"/>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="A157" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E157" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F157" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G157" s="5"/>
+      <c r="H157" s="5"/>
+      <c r="I157" s="5"/>
+      <c r="J157" s="5"/>
+      <c r="K157" s="5"/>
+      <c r="L157" s="5"/>
+      <c r="M157" s="5"/>
+      <c r="N157" s="5"/>
+    </row>
+    <row r="158" spans="1:14">
+      <c r="A158" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B158" s="6">
+        <v>45065</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D158" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E158" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G158" s="9"/>
+      <c r="H158" s="9"/>
+      <c r="I158" s="9"/>
+      <c r="J158" s="9"/>
+      <c r="K158" s="9"/>
+      <c r="L158" s="9"/>
+      <c r="M158" s="9"/>
+      <c r="N158" s="9"/>
+    </row>
+    <row r="159" spans="1:14">
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D159" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E159" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F159" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G159" s="9"/>
+      <c r="H159" s="9"/>
+      <c r="I159" s="9"/>
+      <c r="J159" s="9"/>
+      <c r="K159" s="9"/>
+      <c r="L159" s="9"/>
+      <c r="M159" s="9"/>
+      <c r="N159" s="9"/>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D160" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E160" s="36">
+        <v>0.186111111111111</v>
+      </c>
+      <c r="F160" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G160" s="9"/>
+      <c r="H160" s="9"/>
+      <c r="I160" s="9"/>
+      <c r="J160" s="9"/>
+      <c r="K160" s="9"/>
+      <c r="L160" s="9"/>
+      <c r="M160" s="9"/>
+      <c r="N160" s="9"/>
+    </row>
+    <row r="161" spans="1:14">
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D161" s="36">
+        <v>0.186111111111111</v>
+      </c>
+      <c r="E161" s="36">
+        <v>0.201388888888889</v>
+      </c>
+      <c r="F161" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G161" s="9"/>
+      <c r="H161" s="9"/>
+      <c r="I161" s="9"/>
+      <c r="J161" s="9"/>
+      <c r="K161" s="9"/>
+      <c r="L161" s="9"/>
+      <c r="M161" s="9"/>
+      <c r="N161" s="9"/>
+    </row>
+    <row r="162" spans="1:14">
+      <c r="A162" s="6"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D162" s="36">
+        <v>0.201388888888889</v>
+      </c>
+      <c r="E162" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F162" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="9"/>
+      <c r="J162" s="9"/>
+      <c r="K162" s="9"/>
+      <c r="L162" s="9"/>
+      <c r="M162" s="9"/>
+      <c r="N162" s="9"/>
+    </row>
+    <row r="165" spans="1:14">
+      <c r="A165" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D165" s="16"/>
+      <c r="E165" s="16"/>
+      <c r="F165" s="16"/>
+      <c r="G165" s="16"/>
+      <c r="H165" s="16"/>
+      <c r="I165" s="16"/>
+      <c r="J165" s="16"/>
+      <c r="K165" s="16"/>
+      <c r="L165" s="16"/>
+      <c r="M165" s="16"/>
+      <c r="N165" s="30"/>
+    </row>
+    <row r="166" spans="1:14">
+      <c r="A166" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B166" s="18">
+        <v>45066</v>
+      </c>
+      <c r="C166" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D166" s="20"/>
+      <c r="E166" s="20"/>
+      <c r="F166" s="20"/>
+      <c r="G166" s="20"/>
+      <c r="H166" s="20"/>
+      <c r="I166" s="20"/>
+      <c r="J166" s="20"/>
+      <c r="K166" s="20"/>
+      <c r="L166" s="20"/>
+      <c r="M166" s="20"/>
+      <c r="N166" s="31"/>
+    </row>
+    <row r="167" spans="1:14">
+      <c r="A167" s="21"/>
+      <c r="B167" s="22"/>
+      <c r="C167" s="23"/>
+      <c r="D167" s="24"/>
+      <c r="E167" s="24"/>
+      <c r="F167" s="24"/>
+      <c r="G167" s="24"/>
+      <c r="H167" s="24"/>
+      <c r="I167" s="24"/>
+      <c r="J167" s="24"/>
+      <c r="K167" s="24"/>
+      <c r="L167" s="24"/>
+      <c r="M167" s="24"/>
+      <c r="N167" s="32"/>
+    </row>
+    <row r="168" spans="1:14">
+      <c r="A168" s="25"/>
+      <c r="B168" s="26"/>
+      <c r="C168" s="27"/>
+      <c r="D168" s="28"/>
+      <c r="E168" s="28"/>
+      <c r="F168" s="28"/>
+      <c r="G168" s="28"/>
+      <c r="H168" s="28"/>
+      <c r="I168" s="28"/>
+      <c r="J168" s="28"/>
+      <c r="K168" s="28"/>
+      <c r="L168" s="28"/>
+      <c r="M168" s="28"/>
+      <c r="N168" s="33"/>
+    </row>
+    <row r="169" spans="1:14">
+      <c r="A169" s="29"/>
+      <c r="B169" s="29"/>
+      <c r="C169" s="29"/>
+      <c r="D169" s="29"/>
+      <c r="E169" s="29"/>
+      <c r="F169" s="29"/>
+      <c r="G169" s="29"/>
+      <c r="H169" s="29"/>
+      <c r="I169" s="29"/>
+      <c r="J169" s="29"/>
+      <c r="K169" s="29"/>
+      <c r="L169" s="29"/>
+      <c r="M169" s="29"/>
+      <c r="N169" s="29"/>
+    </row>
+    <row r="170" spans="1:14">
+      <c r="A170" s="29"/>
+      <c r="B170" s="29"/>
+      <c r="C170" s="29"/>
+      <c r="D170" s="29"/>
+      <c r="E170" s="29"/>
+      <c r="F170" s="29"/>
+      <c r="G170" s="29"/>
+      <c r="H170" s="29"/>
+      <c r="I170" s="29"/>
+      <c r="J170" s="29"/>
+      <c r="K170" s="29"/>
+      <c r="L170" s="29"/>
+      <c r="M170" s="29"/>
+      <c r="N170" s="29"/>
+    </row>
+    <row r="171" spans="1:14">
+      <c r="A171" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B171" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D171" s="16"/>
+      <c r="E171" s="16"/>
+      <c r="F171" s="16"/>
+      <c r="G171" s="16"/>
+      <c r="H171" s="16"/>
+      <c r="I171" s="16"/>
+      <c r="J171" s="16"/>
+      <c r="K171" s="16"/>
+      <c r="L171" s="16"/>
+      <c r="M171" s="16"/>
+      <c r="N171" s="30"/>
+    </row>
+    <row r="172" spans="1:14">
+      <c r="A172" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B172" s="18">
+        <v>45067</v>
+      </c>
+      <c r="C172" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D172" s="20"/>
+      <c r="E172" s="20"/>
+      <c r="F172" s="20"/>
+      <c r="G172" s="20"/>
+      <c r="H172" s="20"/>
+      <c r="I172" s="20"/>
+      <c r="J172" s="20"/>
+      <c r="K172" s="20"/>
+      <c r="L172" s="20"/>
+      <c r="M172" s="20"/>
+      <c r="N172" s="31"/>
+    </row>
+    <row r="173" spans="1:14">
+      <c r="A173" s="21"/>
+      <c r="B173" s="22"/>
+      <c r="C173" s="23"/>
+      <c r="D173" s="24"/>
+      <c r="E173" s="24"/>
+      <c r="F173" s="24"/>
+      <c r="G173" s="24"/>
+      <c r="H173" s="24"/>
+      <c r="I173" s="24"/>
+      <c r="J173" s="24"/>
+      <c r="K173" s="24"/>
+      <c r="L173" s="24"/>
+      <c r="M173" s="24"/>
+      <c r="N173" s="32"/>
+    </row>
+    <row r="174" spans="1:14">
+      <c r="A174" s="25"/>
+      <c r="B174" s="26"/>
+      <c r="C174" s="27"/>
+      <c r="D174" s="28"/>
+      <c r="E174" s="28"/>
+      <c r="F174" s="28"/>
+      <c r="G174" s="28"/>
+      <c r="H174" s="28"/>
+      <c r="I174" s="28"/>
+      <c r="J174" s="28"/>
+      <c r="K174" s="28"/>
+      <c r="L174" s="28"/>
+      <c r="M174" s="28"/>
+      <c r="N174" s="33"/>
+    </row>
+    <row r="177" spans="1:14">
+      <c r="A177" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C177" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D177" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E177" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F177" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G177" s="5"/>
+      <c r="H177" s="5"/>
+      <c r="I177" s="5"/>
+      <c r="J177" s="5"/>
+      <c r="K177" s="5"/>
+      <c r="L177" s="5"/>
+      <c r="M177" s="5"/>
+      <c r="N177" s="5"/>
+    </row>
+    <row r="178" spans="1:14">
+      <c r="A178" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B178" s="6">
+        <v>45068</v>
+      </c>
+      <c r="C178" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D178" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E178" s="8">
+        <v>0.409722222222222</v>
+      </c>
+      <c r="F178" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="9"/>
+      <c r="K178" s="9"/>
+      <c r="L178" s="9"/>
+      <c r="M178" s="9"/>
+      <c r="N178" s="9"/>
+    </row>
+    <row r="179" spans="1:14">
+      <c r="A179" s="6"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D179" s="8">
+        <v>0.409722222222222</v>
+      </c>
+      <c r="E179" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F179" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+      <c r="I179" s="9"/>
+      <c r="J179" s="9"/>
+      <c r="K179" s="9"/>
+      <c r="L179" s="9"/>
+      <c r="M179" s="9"/>
+      <c r="N179" s="9"/>
+    </row>
+    <row r="180" spans="1:14">
+      <c r="A180" s="6"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D180" s="8">
+        <v>0.409722222222222</v>
+      </c>
+      <c r="E180" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F180" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+      <c r="I180" s="9"/>
+      <c r="J180" s="9"/>
+      <c r="K180" s="9"/>
+      <c r="L180" s="9"/>
+      <c r="M180" s="9"/>
+      <c r="N180" s="9"/>
+    </row>
+    <row r="181" spans="1:14">
+      <c r="A181" s="6"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D181" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E181" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="F181" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G181" s="9"/>
+      <c r="H181" s="9"/>
+      <c r="I181" s="9"/>
+      <c r="J181" s="9"/>
+      <c r="K181" s="9"/>
+      <c r="L181" s="9"/>
+      <c r="M181" s="9"/>
+      <c r="N181" s="9"/>
+    </row>
+    <row r="182" spans="1:14">
+      <c r="A182" s="6"/>
+      <c r="B182" s="6"/>
+      <c r="C182" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D182" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="E182" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F182" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G182" s="9"/>
+      <c r="H182" s="9"/>
+      <c r="I182" s="9"/>
+      <c r="J182" s="9"/>
+      <c r="K182" s="9"/>
+      <c r="L182" s="9"/>
+      <c r="M182" s="9"/>
+      <c r="N182" s="9"/>
+    </row>
+    <row r="185" spans="1:14">
+      <c r="A185" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D185" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E185" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F185" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G185" s="5"/>
+      <c r="H185" s="5"/>
+      <c r="I185" s="5"/>
+      <c r="J185" s="5"/>
+      <c r="K185" s="5"/>
+      <c r="L185" s="5"/>
+      <c r="M185" s="5"/>
+      <c r="N185" s="5"/>
+    </row>
+    <row r="186" spans="1:14">
+      <c r="A186" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B186" s="6">
+        <v>45069</v>
+      </c>
+      <c r="C186" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D186" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E186" s="8">
+        <v>0.409722222222222</v>
+      </c>
+      <c r="F186" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G186" s="9"/>
+      <c r="H186" s="9"/>
+      <c r="I186" s="9"/>
+      <c r="J186" s="9"/>
+      <c r="K186" s="9"/>
+      <c r="L186" s="9"/>
+      <c r="M186" s="9"/>
+      <c r="N186" s="9"/>
+    </row>
+    <row r="187" spans="1:14">
+      <c r="A187" s="6"/>
+      <c r="B187" s="6"/>
+      <c r="C187" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D187" s="8">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E187" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F187" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G187" s="9"/>
+      <c r="H187" s="9"/>
+      <c r="I187" s="9"/>
+      <c r="J187" s="9"/>
+      <c r="K187" s="9"/>
+      <c r="L187" s="9"/>
+      <c r="M187" s="9"/>
+      <c r="N187" s="9"/>
+    </row>
+    <row r="188" spans="1:14">
+      <c r="A188" s="6"/>
+      <c r="B188" s="6"/>
+      <c r="C188" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D188" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E188" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="F188" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G188" s="9"/>
+      <c r="H188" s="9"/>
+      <c r="I188" s="9"/>
+      <c r="J188" s="9"/>
+      <c r="K188" s="9"/>
+      <c r="L188" s="9"/>
+      <c r="M188" s="9"/>
+      <c r="N188" s="9"/>
+    </row>
+    <row r="189" spans="1:14">
+      <c r="A189" s="6"/>
+      <c r="B189" s="6"/>
+      <c r="C189" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D189" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="E189" s="8">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="F189" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G189" s="9"/>
+      <c r="H189" s="9"/>
+      <c r="I189" s="9"/>
+      <c r="J189" s="9"/>
+      <c r="K189" s="9"/>
+      <c r="L189" s="9"/>
+      <c r="M189" s="9"/>
+      <c r="N189" s="9"/>
+    </row>
+    <row r="190" spans="1:14">
+      <c r="A190" s="6"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D190" s="8">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="E190" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F190" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G190" s="9"/>
+      <c r="H190" s="9"/>
+      <c r="I190" s="9"/>
+      <c r="J190" s="9"/>
+      <c r="K190" s="9"/>
+      <c r="L190" s="9"/>
+      <c r="M190" s="9"/>
+      <c r="N190" s="9"/>
+    </row>
+    <row r="193" spans="1:14">
+      <c r="A193" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C193" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D193" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E193" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G193" s="5"/>
+      <c r="H193" s="5"/>
+      <c r="I193" s="5"/>
+      <c r="J193" s="5"/>
+      <c r="K193" s="5"/>
+      <c r="L193" s="5"/>
+      <c r="M193" s="5"/>
+      <c r="N193" s="5"/>
+    </row>
+    <row r="194" spans="1:14">
+      <c r="A194" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B194" s="6">
+        <v>45070</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D194" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E194" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F194" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G194" s="9"/>
+      <c r="H194" s="9"/>
+      <c r="I194" s="9"/>
+      <c r="J194" s="9"/>
+      <c r="K194" s="9"/>
+      <c r="L194" s="9"/>
+      <c r="M194" s="9"/>
+      <c r="N194" s="9"/>
+    </row>
+    <row r="195" spans="1:14">
+      <c r="A195" s="6"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D195" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E195" s="8">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="F195" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G195" s="9"/>
+      <c r="H195" s="9"/>
+      <c r="I195" s="9"/>
+      <c r="J195" s="9"/>
+      <c r="K195" s="9"/>
+      <c r="L195" s="9"/>
+      <c r="M195" s="9"/>
+      <c r="N195" s="9"/>
+    </row>
+    <row r="196" spans="1:14">
+      <c r="A196" s="6"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D196" s="8">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E196" s="8">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="F196" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G196" s="9"/>
+      <c r="H196" s="9"/>
+      <c r="I196" s="9"/>
+      <c r="J196" s="9"/>
+      <c r="K196" s="9"/>
+      <c r="L196" s="9"/>
+      <c r="M196" s="9"/>
+      <c r="N196" s="9"/>
+    </row>
+    <row r="197" spans="1:14">
+      <c r="A197" s="6"/>
+      <c r="B197" s="6"/>
+      <c r="C197" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D197" s="8">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="E197" s="8">
+        <v>0.493055555555556</v>
+      </c>
+      <c r="F197" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G197" s="9"/>
+      <c r="H197" s="9"/>
+      <c r="I197" s="9"/>
+      <c r="J197" s="9"/>
+      <c r="K197" s="9"/>
+      <c r="L197" s="9"/>
+      <c r="M197" s="9"/>
+      <c r="N197" s="9"/>
+    </row>
+    <row r="198" spans="1:14">
+      <c r="A198" s="6"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D198" s="8">
+        <v>0.493055555555556</v>
+      </c>
+      <c r="E198" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F198" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G198" s="9"/>
+      <c r="H198" s="9"/>
+      <c r="I198" s="9"/>
+      <c r="J198" s="9"/>
+      <c r="K198" s="9"/>
+      <c r="L198" s="9"/>
+      <c r="M198" s="9"/>
+      <c r="N198" s="9"/>
+    </row>
+    <row r="199" spans="1:14">
+      <c r="A199" s="6"/>
+      <c r="B199" s="6"/>
+      <c r="C199" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D199" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E199" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="F199" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G199" s="9"/>
+      <c r="H199" s="9"/>
+      <c r="I199" s="9"/>
+      <c r="J199" s="9"/>
+      <c r="K199" s="9"/>
+      <c r="L199" s="9"/>
+      <c r="M199" s="9"/>
+      <c r="N199" s="9"/>
+    </row>
+    <row r="200" spans="1:14">
+      <c r="A200" s="6"/>
+      <c r="B200" s="6"/>
+      <c r="C200" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D200" s="8">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="E200" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="F200" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G200" s="9"/>
+      <c r="H200" s="9"/>
+      <c r="I200" s="9"/>
+      <c r="J200" s="9"/>
+      <c r="K200" s="9"/>
+      <c r="L200" s="9"/>
+      <c r="M200" s="9"/>
+      <c r="N200" s="9"/>
+    </row>
+    <row r="201" spans="1:14">
+      <c r="A201" s="6"/>
+      <c r="B201" s="6"/>
+      <c r="C201" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D201" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="E201" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F201" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G201" s="9"/>
+      <c r="H201" s="9"/>
+      <c r="I201" s="9"/>
+      <c r="J201" s="9"/>
+      <c r="K201" s="9"/>
+      <c r="L201" s="9"/>
+      <c r="M201" s="9"/>
+      <c r="N201" s="9"/>
+    </row>
+    <row r="205" spans="1:14">
+      <c r="A205" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E205" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F205" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G205" s="5"/>
+      <c r="H205" s="5"/>
+      <c r="I205" s="5"/>
+      <c r="J205" s="5"/>
+      <c r="K205" s="5"/>
+      <c r="L205" s="5"/>
+      <c r="M205" s="5"/>
+      <c r="N205" s="5"/>
+    </row>
+    <row r="206" spans="1:14">
+      <c r="A206" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B206" s="6">
+        <v>45071</v>
+      </c>
+      <c r="C206" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D206" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E206" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F206" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G206" s="9"/>
+      <c r="H206" s="9"/>
+      <c r="I206" s="9"/>
+      <c r="J206" s="9"/>
+      <c r="K206" s="9"/>
+      <c r="L206" s="9"/>
+      <c r="M206" s="9"/>
+      <c r="N206" s="9"/>
+    </row>
+    <row r="207" spans="1:14">
+      <c r="A207" s="6"/>
+      <c r="B207" s="6"/>
+      <c r="C207" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D207" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E207" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="F207" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G207" s="9"/>
+      <c r="H207" s="9"/>
+      <c r="I207" s="9"/>
+      <c r="J207" s="9"/>
+      <c r="K207" s="9"/>
+      <c r="L207" s="9"/>
+      <c r="M207" s="9"/>
+      <c r="N207" s="9"/>
+    </row>
+    <row r="208" spans="1:14">
+      <c r="A208" s="6"/>
+      <c r="B208" s="6"/>
+      <c r="C208" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D208" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="E208" s="8">
+        <v>0.53125</v>
+      </c>
+      <c r="F208" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G208" s="9"/>
+      <c r="H208" s="9"/>
+      <c r="I208" s="9"/>
+      <c r="J208" s="9"/>
+      <c r="K208" s="9"/>
+      <c r="L208" s="9"/>
+      <c r="M208" s="9"/>
+      <c r="N208" s="9"/>
+    </row>
+    <row r="209" spans="1:14">
+      <c r="A209" s="6"/>
+      <c r="B209" s="6"/>
+      <c r="C209" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D209" s="8">
+        <v>0.53125</v>
+      </c>
+      <c r="E209" s="8">
+        <v>0.538194444444444</v>
+      </c>
+      <c r="F209" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G209" s="9"/>
+      <c r="H209" s="9"/>
+      <c r="I209" s="9"/>
+      <c r="J209" s="9"/>
+      <c r="K209" s="9"/>
+      <c r="L209" s="9"/>
+      <c r="M209" s="9"/>
+      <c r="N209" s="9"/>
+    </row>
+    <row r="210" spans="1:14">
+      <c r="A210" s="6"/>
+      <c r="B210" s="6"/>
+      <c r="C210" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D210" s="8">
+        <v>0.538194444444444</v>
+      </c>
+      <c r="E210" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F210" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G210" s="9"/>
+      <c r="H210" s="9"/>
+      <c r="I210" s="9"/>
+      <c r="J210" s="9"/>
+      <c r="K210" s="9"/>
+      <c r="L210" s="9"/>
+      <c r="M210" s="9"/>
+      <c r="N210" s="9"/>
+    </row>
+    <row r="211" spans="1:14">
+      <c r="A211" s="37"/>
+      <c r="B211" s="37"/>
+      <c r="C211" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D211" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E211" s="11">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F211" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G211" s="9"/>
+      <c r="H211" s="9"/>
+      <c r="I211" s="9"/>
+      <c r="J211" s="9"/>
+      <c r="K211" s="9"/>
+      <c r="L211" s="9"/>
+      <c r="M211" s="9"/>
+      <c r="N211" s="9"/>
+    </row>
+    <row r="212" spans="1:14">
+      <c r="A212" s="37"/>
+      <c r="B212" s="37"/>
+      <c r="C212" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D212" s="11">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E212" s="8">
+        <v>0.1875</v>
+      </c>
+      <c r="F212" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="G212" s="39"/>
+      <c r="H212" s="39"/>
+      <c r="I212" s="39"/>
+      <c r="J212" s="39"/>
+      <c r="K212" s="39"/>
+      <c r="L212" s="39"/>
+      <c r="M212" s="39"/>
+      <c r="N212" s="39"/>
+    </row>
+    <row r="213" spans="1:14">
+      <c r="A213" s="37"/>
+      <c r="B213" s="37"/>
+      <c r="C213" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D213" s="8">
+        <v>0.1875</v>
+      </c>
+      <c r="E213" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F213" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G213" s="9"/>
+      <c r="H213" s="9"/>
+      <c r="I213" s="9"/>
+      <c r="J213" s="9"/>
+      <c r="K213" s="9"/>
+      <c r="L213" s="9"/>
+      <c r="M213" s="9"/>
+      <c r="N213" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="141">
+  <mergeCells count="197">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -4357,6 +5676,46 @@
     <mergeCell ref="F150:N150"/>
     <mergeCell ref="F151:N151"/>
     <mergeCell ref="F152:N152"/>
+    <mergeCell ref="F153:N153"/>
+    <mergeCell ref="F154:N154"/>
+    <mergeCell ref="F157:N157"/>
+    <mergeCell ref="F158:N158"/>
+    <mergeCell ref="F159:N159"/>
+    <mergeCell ref="F160:N160"/>
+    <mergeCell ref="F161:N161"/>
+    <mergeCell ref="F162:N162"/>
+    <mergeCell ref="C165:N165"/>
+    <mergeCell ref="C171:N171"/>
+    <mergeCell ref="F177:N177"/>
+    <mergeCell ref="F178:N178"/>
+    <mergeCell ref="F179:N179"/>
+    <mergeCell ref="F180:N180"/>
+    <mergeCell ref="F181:N181"/>
+    <mergeCell ref="F182:N182"/>
+    <mergeCell ref="F185:N185"/>
+    <mergeCell ref="F186:N186"/>
+    <mergeCell ref="F187:N187"/>
+    <mergeCell ref="F188:N188"/>
+    <mergeCell ref="F189:N189"/>
+    <mergeCell ref="F190:N190"/>
+    <mergeCell ref="F193:N193"/>
+    <mergeCell ref="F194:N194"/>
+    <mergeCell ref="F195:N195"/>
+    <mergeCell ref="F196:N196"/>
+    <mergeCell ref="F197:N197"/>
+    <mergeCell ref="F198:N198"/>
+    <mergeCell ref="F199:N199"/>
+    <mergeCell ref="F200:N200"/>
+    <mergeCell ref="F201:N201"/>
+    <mergeCell ref="F205:N205"/>
+    <mergeCell ref="F206:N206"/>
+    <mergeCell ref="F207:N207"/>
+    <mergeCell ref="F208:N208"/>
+    <mergeCell ref="F209:N209"/>
+    <mergeCell ref="F210:N210"/>
+    <mergeCell ref="F211:N211"/>
+    <mergeCell ref="F212:N212"/>
+    <mergeCell ref="F213:N213"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A26:A30"/>
@@ -4374,7 +5733,14 @@
     <mergeCell ref="A119:A124"/>
     <mergeCell ref="A128:A133"/>
     <mergeCell ref="A137:A143"/>
-    <mergeCell ref="A147:A152"/>
+    <mergeCell ref="A147:A154"/>
+    <mergeCell ref="A158:A162"/>
+    <mergeCell ref="A166:A168"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A178:A182"/>
+    <mergeCell ref="A186:A190"/>
+    <mergeCell ref="A194:A201"/>
+    <mergeCell ref="A206:A213"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B26:B30"/>
@@ -4392,7 +5758,14 @@
     <mergeCell ref="B119:B124"/>
     <mergeCell ref="B128:B133"/>
     <mergeCell ref="B137:B143"/>
-    <mergeCell ref="B147:B152"/>
+    <mergeCell ref="B147:B154"/>
+    <mergeCell ref="B158:B162"/>
+    <mergeCell ref="B166:B168"/>
+    <mergeCell ref="B172:B174"/>
+    <mergeCell ref="B178:B182"/>
+    <mergeCell ref="B186:B190"/>
+    <mergeCell ref="B194:B201"/>
+    <mergeCell ref="B206:B213"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C37:C38"/>
@@ -4411,6 +5784,8 @@
     <mergeCell ref="C55:N57"/>
     <mergeCell ref="C107:N109"/>
     <mergeCell ref="C113:N115"/>
+    <mergeCell ref="C166:N168"/>
+    <mergeCell ref="C172:N174"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
31 May DSR  complete Month dsr
Complete Month DSR
</commit_message>
<xml_diff>
--- a/05_may_/May2023.xlsx
+++ b/05_may_/May2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="148">
   <si>
     <t>Day</t>
   </si>
@@ -374,6 +374,90 @@
   </si>
   <si>
     <t>work on the sorting related issue in common nutrition list</t>
+  </si>
+  <si>
+    <t>WBX-4690</t>
+  </si>
+  <si>
+    <t>took clone of wellbux project from official git account N install node modules N migrate code</t>
+  </si>
+  <si>
+    <t>start server check changes and test on the local and raised the pr of it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tried to take a clone of ewh project from official git account </t>
+  </si>
+  <si>
+    <t>walkthrough the garmin code on wellbux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watch tutorial on utube of garmin implementation and walkthrough the code </t>
+  </si>
+  <si>
+    <t>update code and use common validation in common nutrition list</t>
+  </si>
+  <si>
+    <t>WBX-4671</t>
+  </si>
+  <si>
+    <t>figureOut the problem in email verification link during create a user in admin side</t>
+  </si>
+  <si>
+    <t>try to understand implementation of garmin in wbx and saw the code</t>
+  </si>
+  <si>
+    <t>add common services numericOrder sorting for common nutrition list in trackers food</t>
+  </si>
+  <si>
+    <t>WBX-3120</t>
+  </si>
+  <si>
+    <t>ask question from faizan about gamin</t>
+  </si>
+  <si>
+    <t>figure out the and solved the backend listing issue in common nut list</t>
+  </si>
+  <si>
+    <t>install globally localtunnel try to go live but does not work try another one ngrok for live it gives me error and saw the files of garmin codes and implementation</t>
+  </si>
+  <si>
+    <t>Due to Office Cleaning...</t>
+  </si>
+  <si>
+    <t>LMDI-47</t>
+  </si>
+  <si>
+    <t>tried the localhost with localtunnel to live to the internet and through utube video</t>
+  </si>
+  <si>
+    <t>Tried From ngrok for live of localhost and through utube video</t>
+  </si>
+  <si>
+    <t>reivewed pr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify the email link is not come from admin side for create a user </t>
+  </si>
+  <si>
+    <t xml:space="preserve">took credentials  of developer garmin portal and download docs and watch video of gcdp understand the work flow of apis </t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>find a user tried to login who have garmin device linked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reads api documentation and login credentials and create new user </t>
+  </si>
+  <si>
+    <t>discussion with faizan about garmin device and connectivity</t>
+  </si>
+  <si>
+    <t>make connection establish between wbx app to local server for garmin data</t>
+  </si>
+  <si>
+    <t>add new user to garmin device to tried to add data for synchronization</t>
   </si>
 </sst>
 </file>
@@ -381,11 +465,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="mmm/yy"/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="mmm/yy"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="182" formatCode="h:mm"/>
   </numFmts>
@@ -435,6 +519,21 @@
       <charset val="0"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -449,6 +548,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -457,39 +571,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,14 +595,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -531,6 +607,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -556,16 +640,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -610,48 +694,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -664,13 +706,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,55 +736,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -748,25 +784,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,82 +1161,82 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1161,70 +1245,70 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1324,14 +1408,23 @@
     <xf numFmtId="182" fontId="5" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="5" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="5" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="181" fontId="3" fillId="4" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1652,10 +1745,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P213"/>
+  <dimension ref="A1:P272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="R211" sqref="R211"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="J279" sqref="J279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -5516,8 +5609,8 @@
       <c r="N210" s="9"/>
     </row>
     <row r="211" spans="1:14">
-      <c r="A211" s="37"/>
-      <c r="B211" s="37"/>
+      <c r="A211" s="6"/>
+      <c r="B211" s="6"/>
       <c r="C211" s="7" t="s">
         <v>82</v>
       </c>
@@ -5540,9 +5633,9 @@
       <c r="N211" s="9"/>
     </row>
     <row r="212" spans="1:14">
-      <c r="A212" s="37"/>
-      <c r="B212" s="37"/>
-      <c r="C212" s="38" t="s">
+      <c r="A212" s="6"/>
+      <c r="B212" s="6"/>
+      <c r="C212" s="37" t="s">
         <v>39</v>
       </c>
       <c r="D212" s="11">
@@ -5551,21 +5644,21 @@
       <c r="E212" s="8">
         <v>0.1875</v>
       </c>
-      <c r="F212" s="39" t="s">
+      <c r="F212" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="G212" s="39"/>
-      <c r="H212" s="39"/>
-      <c r="I212" s="39"/>
-      <c r="J212" s="39"/>
-      <c r="K212" s="39"/>
-      <c r="L212" s="39"/>
-      <c r="M212" s="39"/>
-      <c r="N212" s="39"/>
+      <c r="G212" s="38"/>
+      <c r="H212" s="38"/>
+      <c r="I212" s="38"/>
+      <c r="J212" s="38"/>
+      <c r="K212" s="38"/>
+      <c r="L212" s="38"/>
+      <c r="M212" s="38"/>
+      <c r="N212" s="38"/>
     </row>
     <row r="213" spans="1:14">
-      <c r="A213" s="37"/>
-      <c r="B213" s="37"/>
+      <c r="A213" s="6"/>
+      <c r="B213" s="6"/>
       <c r="C213" s="7" t="s">
         <v>52</v>
       </c>
@@ -5587,8 +5680,1126 @@
       <c r="M213" s="9"/>
       <c r="N213" s="9"/>
     </row>
+    <row r="217" spans="1:14">
+      <c r="A217" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B217" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C217" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D217" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E217" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F217" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G217" s="5"/>
+      <c r="H217" s="5"/>
+      <c r="I217" s="5"/>
+      <c r="J217" s="5"/>
+      <c r="K217" s="5"/>
+      <c r="L217" s="5"/>
+      <c r="M217" s="5"/>
+      <c r="N217" s="5"/>
+    </row>
+    <row r="218" spans="1:14">
+      <c r="A218" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B218" s="6">
+        <v>45072</v>
+      </c>
+      <c r="C218" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D218" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E218" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F218" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G218" s="9"/>
+      <c r="H218" s="9"/>
+      <c r="I218" s="9"/>
+      <c r="J218" s="9"/>
+      <c r="K218" s="9"/>
+      <c r="L218" s="9"/>
+      <c r="M218" s="9"/>
+      <c r="N218" s="9"/>
+    </row>
+    <row r="219" spans="1:14">
+      <c r="A219" s="6"/>
+      <c r="B219" s="6"/>
+      <c r="C219" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D219" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E219" s="8">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="F219" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G219" s="9"/>
+      <c r="H219" s="9"/>
+      <c r="I219" s="9"/>
+      <c r="J219" s="9"/>
+      <c r="K219" s="9"/>
+      <c r="L219" s="9"/>
+      <c r="M219" s="9"/>
+      <c r="N219" s="9"/>
+    </row>
+    <row r="220" spans="1:14">
+      <c r="A220" s="6"/>
+      <c r="B220" s="6"/>
+      <c r="C220" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D220" s="8">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E220" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="F220" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G220" s="9"/>
+      <c r="H220" s="9"/>
+      <c r="I220" s="9"/>
+      <c r="J220" s="9"/>
+      <c r="K220" s="9"/>
+      <c r="L220" s="9"/>
+      <c r="M220" s="9"/>
+      <c r="N220" s="9"/>
+    </row>
+    <row r="221" spans="1:14">
+      <c r="A221" s="6"/>
+      <c r="B221" s="6"/>
+      <c r="C221" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D221" s="8">
+        <v>0.4375</v>
+      </c>
+      <c r="E221" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F221" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G221" s="9"/>
+      <c r="H221" s="9"/>
+      <c r="I221" s="9"/>
+      <c r="J221" s="9"/>
+      <c r="K221" s="9"/>
+      <c r="L221" s="9"/>
+      <c r="M221" s="9"/>
+      <c r="N221" s="9"/>
+    </row>
+    <row r="222" spans="1:14">
+      <c r="A222" s="6"/>
+      <c r="B222" s="6"/>
+      <c r="C222" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D222" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E222" s="8">
+        <v>0.53125</v>
+      </c>
+      <c r="F222" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G222" s="9"/>
+      <c r="H222" s="9"/>
+      <c r="I222" s="9"/>
+      <c r="J222" s="9"/>
+      <c r="K222" s="9"/>
+      <c r="L222" s="9"/>
+      <c r="M222" s="9"/>
+      <c r="N222" s="9"/>
+    </row>
+    <row r="223" spans="1:14">
+      <c r="A223" s="6"/>
+      <c r="B223" s="6"/>
+      <c r="C223" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D223" s="8">
+        <v>0.53125</v>
+      </c>
+      <c r="E223" s="8">
+        <v>0.534722222222222</v>
+      </c>
+      <c r="F223" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G223" s="9"/>
+      <c r="H223" s="9"/>
+      <c r="I223" s="9"/>
+      <c r="J223" s="9"/>
+      <c r="K223" s="9"/>
+      <c r="L223" s="9"/>
+      <c r="M223" s="9"/>
+      <c r="N223" s="9"/>
+    </row>
+    <row r="224" spans="1:14">
+      <c r="A224" s="6"/>
+      <c r="B224" s="6"/>
+      <c r="C224" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D224" s="8">
+        <v>0.534722222222222</v>
+      </c>
+      <c r="E224" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F224" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G224" s="9"/>
+      <c r="H224" s="9"/>
+      <c r="I224" s="9"/>
+      <c r="J224" s="9"/>
+      <c r="K224" s="9"/>
+      <c r="L224" s="9"/>
+      <c r="M224" s="9"/>
+      <c r="N224" s="9"/>
+    </row>
+    <row r="225" spans="1:14">
+      <c r="A225" s="6"/>
+      <c r="B225" s="6"/>
+      <c r="C225" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D225" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E225" s="11">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F225" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G225" s="9"/>
+      <c r="H225" s="9"/>
+      <c r="I225" s="9"/>
+      <c r="J225" s="9"/>
+      <c r="K225" s="9"/>
+      <c r="L225" s="9"/>
+      <c r="M225" s="9"/>
+      <c r="N225" s="9"/>
+    </row>
+    <row r="226" spans="1:14">
+      <c r="A226" s="6"/>
+      <c r="B226" s="6"/>
+      <c r="C226" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D226" s="11">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E226" s="8">
+        <v>0.21875</v>
+      </c>
+      <c r="F226" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G226" s="9"/>
+      <c r="H226" s="9"/>
+      <c r="I226" s="9"/>
+      <c r="J226" s="9"/>
+      <c r="K226" s="9"/>
+      <c r="L226" s="9"/>
+      <c r="M226" s="9"/>
+      <c r="N226" s="9"/>
+    </row>
+    <row r="227" spans="1:14">
+      <c r="A227" s="6"/>
+      <c r="B227" s="6"/>
+      <c r="C227" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="D227" s="8">
+        <v>0.21875</v>
+      </c>
+      <c r="E227" s="40">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="F227" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="G227" s="38"/>
+      <c r="H227" s="38"/>
+      <c r="I227" s="38"/>
+      <c r="J227" s="38"/>
+      <c r="K227" s="38"/>
+      <c r="L227" s="38"/>
+      <c r="M227" s="38"/>
+      <c r="N227" s="38"/>
+    </row>
+    <row r="228" spans="1:14">
+      <c r="A228" s="6"/>
+      <c r="B228" s="6"/>
+      <c r="C228" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D228" s="40">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="E228" s="40">
+        <v>0.256944444444444</v>
+      </c>
+      <c r="F228" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="G228" s="38"/>
+      <c r="H228" s="38"/>
+      <c r="I228" s="38"/>
+      <c r="J228" s="38"/>
+      <c r="K228" s="38"/>
+      <c r="L228" s="38"/>
+      <c r="M228" s="38"/>
+      <c r="N228" s="38"/>
+    </row>
+    <row r="229" spans="1:14">
+      <c r="A229" s="6"/>
+      <c r="B229" s="6"/>
+      <c r="C229" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D229" s="40">
+        <v>0.256944444444444</v>
+      </c>
+      <c r="E229" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F229" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G229" s="9"/>
+      <c r="H229" s="9"/>
+      <c r="I229" s="9"/>
+      <c r="J229" s="9"/>
+      <c r="K229" s="9"/>
+      <c r="L229" s="9"/>
+      <c r="M229" s="9"/>
+      <c r="N229" s="9"/>
+    </row>
+    <row r="232" spans="1:14">
+      <c r="A232" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B232" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C232" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D232" s="16"/>
+      <c r="E232" s="16"/>
+      <c r="F232" s="16"/>
+      <c r="G232" s="16"/>
+      <c r="H232" s="16"/>
+      <c r="I232" s="16"/>
+      <c r="J232" s="16"/>
+      <c r="K232" s="16"/>
+      <c r="L232" s="16"/>
+      <c r="M232" s="16"/>
+      <c r="N232" s="30"/>
+    </row>
+    <row r="233" spans="1:14">
+      <c r="A233" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B233" s="18">
+        <v>45073</v>
+      </c>
+      <c r="C233" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D233" s="20"/>
+      <c r="E233" s="20"/>
+      <c r="F233" s="20"/>
+      <c r="G233" s="20"/>
+      <c r="H233" s="20"/>
+      <c r="I233" s="20"/>
+      <c r="J233" s="20"/>
+      <c r="K233" s="20"/>
+      <c r="L233" s="20"/>
+      <c r="M233" s="20"/>
+      <c r="N233" s="31"/>
+    </row>
+    <row r="234" spans="1:14">
+      <c r="A234" s="21"/>
+      <c r="B234" s="22"/>
+      <c r="C234" s="23"/>
+      <c r="D234" s="24"/>
+      <c r="E234" s="24"/>
+      <c r="F234" s="24"/>
+      <c r="G234" s="24"/>
+      <c r="H234" s="24"/>
+      <c r="I234" s="24"/>
+      <c r="J234" s="24"/>
+      <c r="K234" s="24"/>
+      <c r="L234" s="24"/>
+      <c r="M234" s="24"/>
+      <c r="N234" s="32"/>
+    </row>
+    <row r="235" spans="1:14">
+      <c r="A235" s="25"/>
+      <c r="B235" s="26"/>
+      <c r="C235" s="27"/>
+      <c r="D235" s="28"/>
+      <c r="E235" s="28"/>
+      <c r="F235" s="28"/>
+      <c r="G235" s="28"/>
+      <c r="H235" s="28"/>
+      <c r="I235" s="28"/>
+      <c r="J235" s="28"/>
+      <c r="K235" s="28"/>
+      <c r="L235" s="28"/>
+      <c r="M235" s="28"/>
+      <c r="N235" s="33"/>
+    </row>
+    <row r="236" spans="1:14">
+      <c r="A236" s="29"/>
+      <c r="B236" s="29"/>
+      <c r="C236" s="29"/>
+      <c r="D236" s="29"/>
+      <c r="E236" s="29"/>
+      <c r="F236" s="29"/>
+      <c r="G236" s="29"/>
+      <c r="H236" s="29"/>
+      <c r="I236" s="29"/>
+      <c r="J236" s="29"/>
+      <c r="K236" s="29"/>
+      <c r="L236" s="29"/>
+      <c r="M236" s="29"/>
+      <c r="N236" s="29"/>
+    </row>
+    <row r="237" spans="1:14">
+      <c r="A237" s="29"/>
+      <c r="B237" s="29"/>
+      <c r="C237" s="29"/>
+      <c r="D237" s="29"/>
+      <c r="E237" s="29"/>
+      <c r="F237" s="29"/>
+      <c r="G237" s="29"/>
+      <c r="H237" s="29"/>
+      <c r="I237" s="29"/>
+      <c r="J237" s="29"/>
+      <c r="K237" s="29"/>
+      <c r="L237" s="29"/>
+      <c r="M237" s="29"/>
+      <c r="N237" s="29"/>
+    </row>
+    <row r="238" spans="1:14">
+      <c r="A238" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B238" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C238" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D238" s="16"/>
+      <c r="E238" s="16"/>
+      <c r="F238" s="16"/>
+      <c r="G238" s="16"/>
+      <c r="H238" s="16"/>
+      <c r="I238" s="16"/>
+      <c r="J238" s="16"/>
+      <c r="K238" s="16"/>
+      <c r="L238" s="16"/>
+      <c r="M238" s="16"/>
+      <c r="N238" s="30"/>
+    </row>
+    <row r="239" spans="1:14">
+      <c r="A239" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B239" s="18">
+        <v>45074</v>
+      </c>
+      <c r="C239" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D239" s="20"/>
+      <c r="E239" s="20"/>
+      <c r="F239" s="20"/>
+      <c r="G239" s="20"/>
+      <c r="H239" s="20"/>
+      <c r="I239" s="20"/>
+      <c r="J239" s="20"/>
+      <c r="K239" s="20"/>
+      <c r="L239" s="20"/>
+      <c r="M239" s="20"/>
+      <c r="N239" s="31"/>
+    </row>
+    <row r="240" spans="1:14">
+      <c r="A240" s="21"/>
+      <c r="B240" s="22"/>
+      <c r="C240" s="23"/>
+      <c r="D240" s="24"/>
+      <c r="E240" s="24"/>
+      <c r="F240" s="24"/>
+      <c r="G240" s="24"/>
+      <c r="H240" s="24"/>
+      <c r="I240" s="24"/>
+      <c r="J240" s="24"/>
+      <c r="K240" s="24"/>
+      <c r="L240" s="24"/>
+      <c r="M240" s="24"/>
+      <c r="N240" s="32"/>
+    </row>
+    <row r="241" spans="1:14">
+      <c r="A241" s="25"/>
+      <c r="B241" s="26"/>
+      <c r="C241" s="27"/>
+      <c r="D241" s="28"/>
+      <c r="E241" s="28"/>
+      <c r="F241" s="28"/>
+      <c r="G241" s="28"/>
+      <c r="H241" s="28"/>
+      <c r="I241" s="28"/>
+      <c r="J241" s="28"/>
+      <c r="K241" s="28"/>
+      <c r="L241" s="28"/>
+      <c r="M241" s="28"/>
+      <c r="N241" s="33"/>
+    </row>
+    <row r="244" spans="1:14">
+      <c r="A244" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B244" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C244" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D244" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E244" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F244" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G244" s="5"/>
+      <c r="H244" s="5"/>
+      <c r="I244" s="5"/>
+      <c r="J244" s="5"/>
+      <c r="K244" s="5"/>
+      <c r="L244" s="5"/>
+      <c r="M244" s="5"/>
+      <c r="N244" s="5"/>
+    </row>
+    <row r="245" spans="1:14">
+      <c r="A245" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B245" s="6">
+        <v>45075</v>
+      </c>
+      <c r="C245" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D245" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E245" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F245" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G245" s="9"/>
+      <c r="H245" s="9"/>
+      <c r="I245" s="9"/>
+      <c r="J245" s="9"/>
+      <c r="K245" s="9"/>
+      <c r="L245" s="9"/>
+      <c r="M245" s="9"/>
+      <c r="N245" s="9"/>
+    </row>
+    <row r="246" spans="1:14">
+      <c r="A246" s="6"/>
+      <c r="B246" s="6"/>
+      <c r="C246" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D246" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E246" s="8">
+        <v>0.430555555555556</v>
+      </c>
+      <c r="F246" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G246" s="9"/>
+      <c r="H246" s="9"/>
+      <c r="I246" s="9"/>
+      <c r="J246" s="9"/>
+      <c r="K246" s="9"/>
+      <c r="L246" s="9"/>
+      <c r="M246" s="9"/>
+      <c r="N246" s="9"/>
+    </row>
+    <row r="247" spans="1:14">
+      <c r="A247" s="6"/>
+      <c r="B247" s="6"/>
+      <c r="C247" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D247" s="8">
+        <v>0.430555555555556</v>
+      </c>
+      <c r="E247" s="8">
+        <v>0.440972222222222</v>
+      </c>
+      <c r="F247" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G247" s="9"/>
+      <c r="H247" s="9"/>
+      <c r="I247" s="9"/>
+      <c r="J247" s="9"/>
+      <c r="K247" s="9"/>
+      <c r="L247" s="9"/>
+      <c r="M247" s="9"/>
+      <c r="N247" s="9"/>
+    </row>
+    <row r="248" spans="1:14">
+      <c r="A248" s="6"/>
+      <c r="B248" s="6"/>
+      <c r="C248" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D248" s="8">
+        <v>0.440972222222222</v>
+      </c>
+      <c r="E248" s="8">
+        <v>0.451388888888889</v>
+      </c>
+      <c r="F248" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="G248" s="9"/>
+      <c r="H248" s="9"/>
+      <c r="I248" s="9"/>
+      <c r="J248" s="9"/>
+      <c r="K248" s="9"/>
+      <c r="L248" s="9"/>
+      <c r="M248" s="9"/>
+      <c r="N248" s="9"/>
+    </row>
+    <row r="249" spans="1:14">
+      <c r="A249" s="6"/>
+      <c r="B249" s="6"/>
+      <c r="C249" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D249" s="8">
+        <v>0.451388888888889</v>
+      </c>
+      <c r="E249" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F249" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G249" s="9"/>
+      <c r="H249" s="9"/>
+      <c r="I249" s="9"/>
+      <c r="J249" s="9"/>
+      <c r="K249" s="9"/>
+      <c r="L249" s="9"/>
+      <c r="M249" s="9"/>
+      <c r="N249" s="9"/>
+    </row>
+    <row r="250" spans="1:14">
+      <c r="A250" s="6"/>
+      <c r="B250" s="6"/>
+      <c r="C250" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D250" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E250" s="11">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F250" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="G250" s="41"/>
+      <c r="H250" s="41"/>
+      <c r="I250" s="41"/>
+      <c r="J250" s="41"/>
+      <c r="K250" s="41"/>
+      <c r="L250" s="41"/>
+      <c r="M250" s="41"/>
+      <c r="N250" s="41"/>
+    </row>
+    <row r="251" spans="1:14">
+      <c r="A251" s="6"/>
+      <c r="B251" s="6"/>
+      <c r="C251" s="11"/>
+      <c r="D251" s="11"/>
+      <c r="E251" s="11"/>
+      <c r="F251" s="41"/>
+      <c r="G251" s="41"/>
+      <c r="H251" s="41"/>
+      <c r="I251" s="41"/>
+      <c r="J251" s="41"/>
+      <c r="K251" s="41"/>
+      <c r="L251" s="41"/>
+      <c r="M251" s="41"/>
+      <c r="N251" s="41"/>
+    </row>
+    <row r="254" spans="1:14">
+      <c r="A254" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C254" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D254" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E254" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F254" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G254" s="5"/>
+      <c r="H254" s="5"/>
+      <c r="I254" s="5"/>
+      <c r="J254" s="5"/>
+      <c r="K254" s="5"/>
+      <c r="L254" s="5"/>
+      <c r="M254" s="5"/>
+      <c r="N254" s="5"/>
+    </row>
+    <row r="255" spans="1:14">
+      <c r="A255" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B255" s="6">
+        <v>45076</v>
+      </c>
+      <c r="C255" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D255" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E255" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="F255" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G255" s="9"/>
+      <c r="H255" s="9"/>
+      <c r="I255" s="9"/>
+      <c r="J255" s="9"/>
+      <c r="K255" s="9"/>
+      <c r="L255" s="9"/>
+      <c r="M255" s="9"/>
+      <c r="N255" s="9"/>
+    </row>
+    <row r="256" spans="1:14">
+      <c r="A256" s="6"/>
+      <c r="B256" s="6"/>
+      <c r="C256" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D256" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="E256" s="8">
+        <v>0.447916666666667</v>
+      </c>
+      <c r="F256" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G256" s="9"/>
+      <c r="H256" s="9"/>
+      <c r="I256" s="9"/>
+      <c r="J256" s="9"/>
+      <c r="K256" s="9"/>
+      <c r="L256" s="9"/>
+      <c r="M256" s="9"/>
+      <c r="N256" s="9"/>
+    </row>
+    <row r="257" spans="1:14">
+      <c r="A257" s="6"/>
+      <c r="B257" s="6"/>
+      <c r="C257" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D257" s="8">
+        <v>0.447916666666667</v>
+      </c>
+      <c r="E257" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F257" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G257" s="9"/>
+      <c r="H257" s="9"/>
+      <c r="I257" s="9"/>
+      <c r="J257" s="9"/>
+      <c r="K257" s="9"/>
+      <c r="L257" s="9"/>
+      <c r="M257" s="9"/>
+      <c r="N257" s="9"/>
+    </row>
+    <row r="258" spans="1:14">
+      <c r="A258" s="6"/>
+      <c r="B258" s="6"/>
+      <c r="C258" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D258" s="8">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E258" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F258" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G258" s="9"/>
+      <c r="H258" s="9"/>
+      <c r="I258" s="9"/>
+      <c r="J258" s="9"/>
+      <c r="K258" s="9"/>
+      <c r="L258" s="9"/>
+      <c r="M258" s="9"/>
+      <c r="N258" s="9"/>
+    </row>
+    <row r="259" spans="1:14">
+      <c r="A259" s="6"/>
+      <c r="B259" s="6"/>
+      <c r="C259" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D259" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E259" s="11">
+        <v>0.100694444444444</v>
+      </c>
+      <c r="F259" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G259" s="9"/>
+      <c r="H259" s="9"/>
+      <c r="I259" s="9"/>
+      <c r="J259" s="9"/>
+      <c r="K259" s="9"/>
+      <c r="L259" s="9"/>
+      <c r="M259" s="9"/>
+      <c r="N259" s="9"/>
+    </row>
+    <row r="260" spans="1:14">
+      <c r="A260" s="6"/>
+      <c r="B260" s="6"/>
+      <c r="C260" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D260" s="11">
+        <v>0.100694444444444</v>
+      </c>
+      <c r="E260" s="11">
+        <v>0.114583333333333</v>
+      </c>
+      <c r="F260" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="G260" s="41"/>
+      <c r="H260" s="41"/>
+      <c r="I260" s="41"/>
+      <c r="J260" s="41"/>
+      <c r="K260" s="41"/>
+      <c r="L260" s="41"/>
+      <c r="M260" s="41"/>
+      <c r="N260" s="41"/>
+    </row>
+    <row r="261" spans="1:14">
+      <c r="A261" s="6"/>
+      <c r="B261" s="6"/>
+      <c r="C261" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="D261" s="11">
+        <v>0.114583333333333</v>
+      </c>
+      <c r="E261" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="F261" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="G261" s="41"/>
+      <c r="H261" s="41"/>
+      <c r="I261" s="41"/>
+      <c r="J261" s="41"/>
+      <c r="K261" s="41"/>
+      <c r="L261" s="41"/>
+      <c r="M261" s="41"/>
+      <c r="N261" s="41"/>
+    </row>
+    <row r="262" spans="1:14">
+      <c r="A262" s="6"/>
+      <c r="B262" s="6"/>
+      <c r="C262" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D262" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="E262" s="11">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F262" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="G262" s="41"/>
+      <c r="H262" s="41"/>
+      <c r="I262" s="41"/>
+      <c r="J262" s="41"/>
+      <c r="K262" s="41"/>
+      <c r="L262" s="41"/>
+      <c r="M262" s="41"/>
+      <c r="N262" s="41"/>
+    </row>
+    <row r="263" spans="1:16">
+      <c r="A263" s="6"/>
+      <c r="B263" s="6"/>
+      <c r="C263" s="35"/>
+      <c r="D263" s="11"/>
+      <c r="E263" s="11"/>
+      <c r="F263" s="41"/>
+      <c r="G263" s="41"/>
+      <c r="H263" s="41"/>
+      <c r="I263" s="41"/>
+      <c r="J263" s="41"/>
+      <c r="K263" s="41"/>
+      <c r="L263" s="41"/>
+      <c r="M263" s="41"/>
+      <c r="N263" s="41"/>
+      <c r="P263" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="266" spans="1:14">
+      <c r="A266" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D266" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E266" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F266" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G266" s="5"/>
+      <c r="H266" s="5"/>
+      <c r="I266" s="5"/>
+      <c r="J266" s="5"/>
+      <c r="K266" s="5"/>
+      <c r="L266" s="5"/>
+      <c r="M266" s="5"/>
+      <c r="N266" s="5"/>
+    </row>
+    <row r="267" spans="1:14">
+      <c r="A267" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B267" s="6">
+        <v>45077</v>
+      </c>
+      <c r="C267" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D267" s="8">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E267" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F267" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G267" s="9"/>
+      <c r="H267" s="9"/>
+      <c r="I267" s="9"/>
+      <c r="J267" s="9"/>
+      <c r="K267" s="9"/>
+      <c r="L267" s="9"/>
+      <c r="M267" s="9"/>
+      <c r="N267" s="9"/>
+    </row>
+    <row r="268" spans="1:14">
+      <c r="A268" s="6"/>
+      <c r="B268" s="6"/>
+      <c r="C268" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D268" s="8">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E268" s="8">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="F268" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G268" s="9"/>
+      <c r="H268" s="9"/>
+      <c r="I268" s="9"/>
+      <c r="J268" s="9"/>
+      <c r="K268" s="9"/>
+      <c r="L268" s="9"/>
+      <c r="M268" s="9"/>
+      <c r="N268" s="9"/>
+    </row>
+    <row r="269" spans="1:14">
+      <c r="A269" s="6"/>
+      <c r="B269" s="6"/>
+      <c r="C269" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D269" s="8">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E269" s="8">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F269" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G269" s="9"/>
+      <c r="H269" s="9"/>
+      <c r="I269" s="9"/>
+      <c r="J269" s="9"/>
+      <c r="K269" s="9"/>
+      <c r="L269" s="9"/>
+      <c r="M269" s="9"/>
+      <c r="N269" s="9"/>
+    </row>
+    <row r="270" spans="1:14">
+      <c r="A270" s="6"/>
+      <c r="B270" s="6"/>
+      <c r="C270" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D270" s="11">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E270" s="11">
+        <v>0.09375</v>
+      </c>
+      <c r="F270" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G270" s="9"/>
+      <c r="H270" s="9"/>
+      <c r="I270" s="9"/>
+      <c r="J270" s="9"/>
+      <c r="K270" s="9"/>
+      <c r="L270" s="9"/>
+      <c r="M270" s="9"/>
+      <c r="N270" s="9"/>
+    </row>
+    <row r="271" spans="1:16">
+      <c r="A271" s="6"/>
+      <c r="B271" s="6"/>
+      <c r="C271" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D271" s="11">
+        <v>0.09375</v>
+      </c>
+      <c r="E271" s="8">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F271" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G271" s="9"/>
+      <c r="H271" s="9"/>
+      <c r="I271" s="9"/>
+      <c r="J271" s="9"/>
+      <c r="K271" s="9"/>
+      <c r="L271" s="9"/>
+      <c r="M271" s="9"/>
+      <c r="N271" s="9"/>
+      <c r="P271" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="272" spans="1:14">
+      <c r="A272" s="42"/>
+      <c r="B272" s="42"/>
+      <c r="C272" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D272" s="8">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E272" s="8">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F272" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G272" s="9"/>
+      <c r="H272" s="9"/>
+      <c r="I272" s="9"/>
+      <c r="J272" s="9"/>
+      <c r="K272" s="9"/>
+      <c r="L272" s="9"/>
+      <c r="M272" s="9"/>
+      <c r="N272" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="197">
+  <mergeCells count="255">
     <mergeCell ref="F8:N8"/>
     <mergeCell ref="F9:N9"/>
     <mergeCell ref="F10:N10"/>
@@ -5716,6 +6927,42 @@
     <mergeCell ref="F211:N211"/>
     <mergeCell ref="F212:N212"/>
     <mergeCell ref="F213:N213"/>
+    <mergeCell ref="F217:N217"/>
+    <mergeCell ref="F218:N218"/>
+    <mergeCell ref="F219:N219"/>
+    <mergeCell ref="F220:N220"/>
+    <mergeCell ref="F221:N221"/>
+    <mergeCell ref="F222:N222"/>
+    <mergeCell ref="F223:N223"/>
+    <mergeCell ref="F224:N224"/>
+    <mergeCell ref="F225:N225"/>
+    <mergeCell ref="F226:N226"/>
+    <mergeCell ref="F227:N227"/>
+    <mergeCell ref="F228:N228"/>
+    <mergeCell ref="F229:N229"/>
+    <mergeCell ref="C232:N232"/>
+    <mergeCell ref="C238:N238"/>
+    <mergeCell ref="F244:N244"/>
+    <mergeCell ref="F245:N245"/>
+    <mergeCell ref="F246:N246"/>
+    <mergeCell ref="F247:N247"/>
+    <mergeCell ref="F248:N248"/>
+    <mergeCell ref="F249:N249"/>
+    <mergeCell ref="F254:N254"/>
+    <mergeCell ref="F255:N255"/>
+    <mergeCell ref="F256:N256"/>
+    <mergeCell ref="F257:N257"/>
+    <mergeCell ref="F258:N258"/>
+    <mergeCell ref="F259:N259"/>
+    <mergeCell ref="F260:N260"/>
+    <mergeCell ref="F261:N261"/>
+    <mergeCell ref="F266:N266"/>
+    <mergeCell ref="F267:N267"/>
+    <mergeCell ref="F268:N268"/>
+    <mergeCell ref="F269:N269"/>
+    <mergeCell ref="F270:N270"/>
+    <mergeCell ref="F271:N271"/>
+    <mergeCell ref="F272:N272"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A26:A30"/>
@@ -5741,6 +6988,12 @@
     <mergeCell ref="A186:A190"/>
     <mergeCell ref="A194:A201"/>
     <mergeCell ref="A206:A213"/>
+    <mergeCell ref="A218:A229"/>
+    <mergeCell ref="A233:A235"/>
+    <mergeCell ref="A239:A241"/>
+    <mergeCell ref="A245:A251"/>
+    <mergeCell ref="A255:A263"/>
+    <mergeCell ref="A267:A272"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B22"/>
     <mergeCell ref="B26:B30"/>
@@ -5766,15 +7019,27 @@
     <mergeCell ref="B186:B190"/>
     <mergeCell ref="B194:B201"/>
     <mergeCell ref="B206:B213"/>
+    <mergeCell ref="B218:B229"/>
+    <mergeCell ref="B233:B235"/>
+    <mergeCell ref="B239:B241"/>
+    <mergeCell ref="B245:B251"/>
+    <mergeCell ref="B255:B263"/>
+    <mergeCell ref="B267:B272"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C250:C251"/>
+    <mergeCell ref="C262:C263"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D250:D251"/>
+    <mergeCell ref="D262:D263"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E250:E251"/>
+    <mergeCell ref="E262:E263"/>
     <mergeCell ref="C3:J4"/>
     <mergeCell ref="F11:N12"/>
     <mergeCell ref="F21:N22"/>
@@ -5786,6 +7051,10 @@
     <mergeCell ref="C113:N115"/>
     <mergeCell ref="C166:N168"/>
     <mergeCell ref="C172:N174"/>
+    <mergeCell ref="C233:N235"/>
+    <mergeCell ref="C239:N241"/>
+    <mergeCell ref="F250:N251"/>
+    <mergeCell ref="F262:N263"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>